<commit_message>
<:construction:> adding amortization table
</commit_message>
<xml_diff>
--- a/TOE_Chart.xlsx
+++ b/TOE_Chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drewc\Documents\CIS 036\StudentLoanCalculatorSolution\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3973530F-4D59-4B14-BA8D-47B18B78C692}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B10BD730-3D08-4EBA-8462-F7C655AA0D58}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="6096" xr2:uid="{BA7B75F5-DFC3-438F-B577-52D12EC034DB}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="6090" xr2:uid="{BA7B75F5-DFC3-438F-B577-52D12EC034DB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -209,18 +209,6 @@
   </cellStyleXfs>
   <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -265,6 +253,18 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -583,136 +583,136 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="25.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="25.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.21875" style="15"/>
-    <col min="2" max="2" width="25.21875" style="16"/>
-    <col min="3" max="3" width="25.21875" style="17"/>
+    <col min="1" max="1" width="25.28515625" style="11"/>
+    <col min="2" max="2" width="25.28515625" style="12"/>
+    <col min="3" max="3" width="25.28515625" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:3" s="19" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="18" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="15" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="15" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="8" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="15" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="8" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="15" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="8" t="s">
+    <row r="6" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="15" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="8"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="7"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="8"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="7"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="8"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="7"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="8"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="7"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="8"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="7"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="9"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="11"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="9"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="11"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="9"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="11"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="9"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="11"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="9"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="11"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="12"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="14"/>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="3"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="3"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="3"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="3"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="3"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="7"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="5"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="7"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="5"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="7"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="5"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="7"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="5"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="7"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="8"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>